<commit_message>
PPT extraction successful, UX improvement pending
</commit_message>
<xml_diff>
--- a/output/marchmarketing_summary.xlsx
+++ b/output/marchmarketing_summary.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Posts" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$K$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$K$43</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -539,8 +539,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>Daily Essentials Grab
-[17/02]</t>
+          <t>Weekend Shopping Spree [03/02]</t>
         </is>
       </c>
       <c r="E2" s="4" t="n">
@@ -572,32 +571,30 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>Weekend Shopping Spree [03/02]</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>44105</v>
-      </c>
-      <c r="F3" s="4" t="inlineStr"/>
-      <c r="G3" s="4" t="n">
-        <v>3418</v>
-      </c>
+          <t>KOL TikTok – Nina Tomyam Seafood Recipe [07/02]</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr"/>
+      <c r="F3" s="4" t="n">
+        <v>58652</v>
+      </c>
+      <c r="G3" s="4" t="inlineStr"/>
       <c r="H3" s="4" t="n">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="I3" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J3" s="4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K3" s="4" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -639,254 +636,263 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Daily Essentials Grab
+[17/02]</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>44105</v>
+      </c>
+      <c r="F5" s="4" t="inlineStr"/>
+      <c r="G5" s="4" t="n">
+        <v>3418</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>241</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>KOL TikTok – Nina Cucur Udang Rangup [24/02]</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr"/>
+      <c r="F6" s="4" t="n">
+        <v>55705</v>
+      </c>
+      <c r="G6" s="4" t="inlineStr"/>
+      <c r="H6" s="4" t="n">
+        <v>142</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="J6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>Loyalty Program (Gorme Omura Knife Series) [25/02]</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>42212</v>
+      </c>
+      <c r="F7" s="4" t="inlineStr"/>
+      <c r="G7" s="4" t="n">
+        <v>3391</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>337</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="B8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Post</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>Weekend Shopping Spree 
+[03/02]</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>11692</v>
+      </c>
+      <c r="F8" s="4" t="inlineStr"/>
+      <c r="G8" s="4" t="n">
+        <v>1008</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I8" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>Loyalty Program (Gorme Omura Knife Series) [11/02]</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>12157</v>
+      </c>
+      <c r="F9" s="4" t="inlineStr"/>
+      <c r="G9" s="4" t="n">
+        <v>1002</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>952</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>Daily Essential Grab 
+[17/02]</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>12450</v>
+      </c>
+      <c r="F10" s="4" t="inlineStr"/>
+      <c r="G10" s="4" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>1021</v>
+      </c>
+      <c r="I10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>Promo Cahaya Ramadan
 [26/02]</t>
         </is>
       </c>
-      <c r="E5" s="4" t="n">
-        <v>11692</v>
-      </c>
-      <c r="F5" s="4" t="inlineStr"/>
-      <c r="G5" s="4" t="n">
-        <v>1008</v>
-      </c>
-      <c r="H5" s="4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>Weekend Shopping Spree 
-[03/02]</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr"/>
-      <c r="F6" s="4" t="n">
-        <v>35810</v>
-      </c>
-      <c r="G6" s="4" t="inlineStr"/>
-      <c r="H6" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="I6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>Daily Essential Grab 
-[17/02]</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>12450</v>
-      </c>
-      <c r="F7" s="4" t="inlineStr"/>
-      <c r="G7" s="4" t="n">
-        <v>1025</v>
-      </c>
-      <c r="H7" s="4" t="n">
-        <v>1021</v>
-      </c>
-      <c r="I7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Quesha Back To School Promo [03/02]</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="inlineStr"/>
-      <c r="F8" s="4" t="n">
-        <v>17343</v>
-      </c>
-      <c r="G8" s="4" t="inlineStr"/>
-      <c r="H8" s="4" t="n">
-        <v>180</v>
-      </c>
-      <c r="I8" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J8" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" s="4" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Nina Tomyam Seafood Recipe [07/02]</t>
-        </is>
-      </c>
-      <c r="E9" s="4" t="inlineStr"/>
-      <c r="F9" s="4" t="n">
-        <v>19125</v>
-      </c>
-      <c r="G9" s="4" t="inlineStr"/>
-      <c r="H9" s="4" t="n">
-        <v>461</v>
-      </c>
-      <c r="I9" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="J9" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="K9" s="4" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Saida Back To School / Promosi Ahli [10/02]</t>
-        </is>
-      </c>
-      <c r="E10" s="4" t="inlineStr"/>
-      <c r="F10" s="4" t="n">
-        <v>22053</v>
-      </c>
-      <c r="G10" s="4" t="inlineStr"/>
-      <c r="H10" s="4" t="n">
-        <v>42</v>
-      </c>
-      <c r="I10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Anne Weekend Groceries Shopping [10/02]</t>
-        </is>
-      </c>
-      <c r="E11" s="4" t="inlineStr"/>
-      <c r="F11" s="4" t="n">
-        <v>28764</v>
-      </c>
-      <c r="G11" s="4" t="inlineStr"/>
+      <c r="E11" s="4" t="n">
+        <v>12913</v>
+      </c>
+      <c r="F11" s="4" t="inlineStr"/>
+      <c r="G11" s="4" t="n">
+        <v>1023</v>
+      </c>
       <c r="H11" s="4" t="n">
-        <v>115</v>
+        <v>1017</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J11" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K11" s="4" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
@@ -894,7 +900,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
@@ -903,33 +909,33 @@
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>TikTok ASMR – Restock Pantry [14/02]</t>
+          <t>KOL TikTok – Quesha Back To School Promo [03/02]</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr"/>
       <c r="F12" s="4" t="n">
-        <v>23571</v>
+        <v>17343</v>
       </c>
       <c r="G12" s="4" t="inlineStr"/>
       <c r="H12" s="4" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J12" s="4" t="n">
         <v>2</v>
       </c>
       <c r="K12" s="4" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
@@ -938,33 +944,33 @@
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>KOL TikTok – Wana Grocery Shopping with 2 Kids [17/02]</t>
+          <t>KOL TikTok – Nina Tomyam Seafood Recipe [07/02]</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr"/>
       <c r="F13" s="4" t="n">
-        <v>23214</v>
+        <v>19125</v>
       </c>
       <c r="G13" s="4" t="inlineStr"/>
       <c r="H13" s="4" t="n">
-        <v>69</v>
+        <v>461</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J13" s="4" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K13" s="4" t="n">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
@@ -973,16 +979,16 @@
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>TikTok Video – Dua Lipa Trend [24/02]</t>
+          <t>KOL TikTok – Saida Back To School / Promosi Ahli [10/02]</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr"/>
       <c r="F14" s="4" t="n">
-        <v>45424</v>
+        <v>22053</v>
       </c>
       <c r="G14" s="4" t="inlineStr"/>
       <c r="H14" s="4" t="n">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="I14" s="4" t="n">
         <v>1</v>
@@ -991,15 +997,15 @@
         <v>0</v>
       </c>
       <c r="K14" s="4" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
@@ -1008,33 +1014,33 @@
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>KOL TikTok – Nina Cucur Udang Rangup [24/02]</t>
+          <t>KOL TikTok – Anne Weekend Groceries Shopping [10/02]</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr"/>
       <c r="F15" s="4" t="n">
-        <v>12631</v>
+        <v>28764</v>
       </c>
       <c r="G15" s="4" t="inlineStr"/>
       <c r="H15" s="4" t="n">
-        <v>382</v>
+        <v>115</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J15" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K15" s="4" t="n">
-        <v>50</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
@@ -1043,67 +1049,65 @@
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>TikTok Video – TFVM ada Produk Sendiri [26/02]</t>
+          <t>TikTok ASMR – Restock Pantry [14/02]</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr"/>
       <c r="F16" s="4" t="n">
-        <v>22018</v>
+        <v>23571</v>
       </c>
       <c r="G16" s="4" t="inlineStr"/>
       <c r="H16" s="4" t="n">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J16" s="4" t="n">
         <v>2</v>
       </c>
       <c r="K16" s="4" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>Weekend Shopping Spree [03/02]</t>
-        </is>
-      </c>
-      <c r="E17" s="4" t="n">
-        <v>49275</v>
-      </c>
-      <c r="F17" s="4" t="inlineStr"/>
-      <c r="G17" s="4" t="n">
-        <v>4306</v>
-      </c>
+          <t>KOL TikTok – Wana Grocery Shopping with 2 Kids [17/02]</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr"/>
+      <c r="F17" s="4" t="n">
+        <v>23214</v>
+      </c>
+      <c r="G17" s="4" t="inlineStr"/>
       <c r="H17" s="4" t="n">
-        <v>237</v>
+        <v>69</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J17" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="4" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>2</v>
@@ -1115,33 +1119,33 @@
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>Loyalty Program – Gorme Omura Knife Series [11/02]</t>
+          <t>TikTok Video – Dua Lipa Trend [24/02]</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr"/>
       <c r="F18" s="4" t="n">
-        <v>131496</v>
+        <v>45424</v>
       </c>
       <c r="G18" s="4" t="inlineStr"/>
       <c r="H18" s="4" t="n">
-        <v>481</v>
+        <v>89</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="J18" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K18" s="4" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
@@ -1150,88 +1154,88 @@
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>TikTok Video – Dua Lipa Trend [24/02]</t>
+          <t>KOL TikTok – Nina Cucur Udang Rangup [24/02]</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr"/>
       <c r="F19" s="4" t="n">
-        <v>50440</v>
+        <v>12631</v>
       </c>
       <c r="G19" s="4" t="inlineStr"/>
       <c r="H19" s="4" t="n">
-        <v>33</v>
+        <v>382</v>
       </c>
       <c r="I19" s="4" t="n">
         <v>2</v>
       </c>
       <c r="J19" s="4" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K19" s="4" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>Loyalty Program – Gorme Omura Knife Series [25/02]</t>
-        </is>
-      </c>
-      <c r="E20" s="4" t="n">
-        <v>41788</v>
-      </c>
-      <c r="F20" s="4" t="inlineStr"/>
-      <c r="G20" s="4" t="n">
-        <v>4215</v>
-      </c>
+          <t>TikTok Video – TFVM ada Produk Sendiri [26/02]</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr"/>
+      <c r="F20" s="4" t="n">
+        <v>22018</v>
+      </c>
+      <c r="G20" s="4" t="inlineStr"/>
       <c r="H20" s="4" t="n">
-        <v>268</v>
+        <v>38</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J20" s="4" t="n">
         <v>2</v>
       </c>
       <c r="K20" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>Promo Video: Cahaya Ramadan [26/02]</t>
-        </is>
-      </c>
-      <c r="E21" s="4" t="inlineStr"/>
-      <c r="F21" s="4" t="n">
-        <v>50582</v>
-      </c>
-      <c r="G21" s="4" t="inlineStr"/>
+          <t>Weekend Shopping Spree [03/02]</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="n">
+        <v>49275</v>
+      </c>
+      <c r="F21" s="4" t="inlineStr"/>
+      <c r="G21" s="4" t="n">
+        <v>4306</v>
+      </c>
       <c r="H21" s="4" t="n">
-        <v>34</v>
+        <v>237</v>
       </c>
       <c r="I21" s="4" t="n">
         <v>1</v>
@@ -1240,50 +1244,52 @@
         <v>0</v>
       </c>
       <c r="K21" s="4" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>Quesha: Back to School [03/02]</t>
-        </is>
-      </c>
-      <c r="E22" s="4" t="inlineStr"/>
-      <c r="F22" s="4" t="n">
-        <v>10307</v>
-      </c>
-      <c r="G22" s="4" t="inlineStr"/>
+          <t>Weekend Shopping Spree [03/02]</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v>41113</v>
+      </c>
+      <c r="F22" s="4" t="inlineStr"/>
+      <c r="G22" s="4" t="n">
+        <v>3558</v>
+      </c>
       <c r="H22" s="4" t="n">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="I22" s="4" t="n">
         <v>9</v>
       </c>
       <c r="J22" s="4" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="K22" s="4" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
@@ -1292,103 +1298,107 @@
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>Nina: Tomyam Seafood Recipe [07/02]</t>
+          <t>Nina Tomyam Seafood Recipe [07/02]</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr"/>
       <c r="F23" s="4" t="n">
-        <v>35536</v>
+        <v>131496</v>
       </c>
       <c r="G23" s="4" t="inlineStr"/>
       <c r="H23" s="4" t="n">
-        <v>605</v>
+        <v>481</v>
       </c>
       <c r="I23" s="4" t="n">
-        <v>658</v>
+        <v>21</v>
       </c>
       <c r="J23" s="4" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="K23" s="4" t="n">
-        <v>252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>Saida: Back to School/ Promosi Ahli [10/02]</t>
-        </is>
-      </c>
-      <c r="E24" s="4" t="inlineStr"/>
-      <c r="F24" s="4" t="n">
-        <v>3253</v>
-      </c>
-      <c r="G24" s="4" t="inlineStr"/>
+          <t>Loyalty Program – Gorme Omura Knife Series [11/02]</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="n">
+        <v>47133</v>
+      </c>
+      <c r="F24" s="4" t="inlineStr"/>
+      <c r="G24" s="4" t="n">
+        <v>4132</v>
+      </c>
       <c r="H24" s="4" t="n">
-        <v>326</v>
+        <v>496</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="J24" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K24" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>Wana: Grocery Shopping with 2 Kids [15/02]</t>
-        </is>
-      </c>
-      <c r="E25" s="4" t="inlineStr"/>
-      <c r="F25" s="4" t="n">
-        <v>2186</v>
-      </c>
-      <c r="G25" s="4" t="inlineStr"/>
+          <t>Loyalty Program – Gorme Omura Knife Series [11/02]</t>
+        </is>
+      </c>
+      <c r="E25" s="4" t="n">
+        <v>44547</v>
+      </c>
+      <c r="F25" s="4" t="inlineStr"/>
+      <c r="G25" s="4" t="n">
+        <v>3408</v>
+      </c>
       <c r="H25" s="4" t="n">
-        <v>127</v>
+        <v>470</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J25" s="4" t="n">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K25" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
@@ -1397,104 +1407,640 @@
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>Nina: Cucur Udang Rangup [24/02]</t>
+          <t>TikTok ASMR – Restock Pantry [14/02]</t>
         </is>
       </c>
       <c r="E26" s="4" t="inlineStr"/>
       <c r="F26" s="4" t="n">
-        <v>42767</v>
+        <v>51093</v>
       </c>
       <c r="G26" s="4" t="inlineStr"/>
       <c r="H26" s="4" t="n">
-        <v>694</v>
+        <v>81</v>
       </c>
       <c r="I26" s="4" t="n">
-        <v>299</v>
+        <v>0</v>
       </c>
       <c r="J26" s="4" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="K26" s="4" t="n">
-        <v>791</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>Daily Essential Grab [22/02]</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="n">
+        <v>40740</v>
+      </c>
+      <c r="F27" s="4" t="inlineStr"/>
+      <c r="G27" s="4" t="n">
+        <v>3350</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>88</v>
+      </c>
+      <c r="I27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>Daily Essential Grab [22/02]</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="n">
+        <v>42339</v>
+      </c>
+      <c r="F28" s="4" t="inlineStr"/>
+      <c r="G28" s="4" t="n">
+        <v>3425</v>
+      </c>
+      <c r="H28" s="4" t="n">
+        <v>184</v>
+      </c>
+      <c r="I28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>Nina – Cucur Udang Rangup [24/02]</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr"/>
+      <c r="F29" s="4" t="n">
+        <v>50440</v>
+      </c>
+      <c r="G29" s="4" t="inlineStr"/>
+      <c r="H29" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I29" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>TikTok Video – Dua Lipa Trend [24/02]</t>
+        </is>
+      </c>
+      <c r="E30" s="4" t="inlineStr"/>
+      <c r="F30" s="4" t="n">
+        <v>50719</v>
+      </c>
+      <c r="G30" s="4" t="inlineStr"/>
+      <c r="H30" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>Loyalty Program – Gorme Omura Knife Series [25/02]</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="n">
+        <v>41788</v>
+      </c>
+      <c r="F31" s="4" t="inlineStr"/>
+      <c r="G31" s="4" t="n">
+        <v>4215</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <v>268</v>
+      </c>
+      <c r="I31" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K31" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>Loyalty Program – Gorme Omura Knife Series [25/02]</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="n">
+        <v>42824</v>
+      </c>
+      <c r="F32" s="4" t="inlineStr"/>
+      <c r="G32" s="4" t="n">
+        <v>3395</v>
+      </c>
+      <c r="H32" s="4" t="n">
+        <v>353</v>
+      </c>
+      <c r="I32" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J32" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="K32" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>TikTok Video – TFVM ada Produk Sendiri [26/02]</t>
+        </is>
+      </c>
+      <c r="E33" s="4" t="inlineStr"/>
+      <c r="F33" s="4" t="n">
+        <v>50582</v>
+      </c>
+      <c r="G33" s="4" t="inlineStr"/>
+      <c r="H33" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D34" s="3" t="inlineStr">
+        <is>
+          <t>Promo Video: Cahaya Ramadan [26/02]</t>
+        </is>
+      </c>
+      <c r="E34" s="4" t="inlineStr"/>
+      <c r="F34" s="4" t="n">
+        <v>51285</v>
+      </c>
+      <c r="G34" s="4" t="inlineStr"/>
+      <c r="H34" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>Promo Video: Cahaya Ramadan [26/02]</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="inlineStr"/>
+      <c r="F35" s="4" t="n">
+        <v>50209</v>
+      </c>
+      <c r="G35" s="4" t="inlineStr"/>
+      <c r="H35" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I35" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="inlineStr">
+        <is>
+          <t>Quesha: Back to School [03/02]</t>
+        </is>
+      </c>
+      <c r="E36" s="4" t="inlineStr"/>
+      <c r="F36" s="4" t="n">
+        <v>10307</v>
+      </c>
+      <c r="G36" s="4" t="inlineStr"/>
+      <c r="H36" s="4" t="n">
+        <v>225</v>
+      </c>
+      <c r="I36" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="J36" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="K36" s="4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>Nina: Tomyam Seafood Recipe [07/02]</t>
+        </is>
+      </c>
+      <c r="E37" s="4" t="inlineStr"/>
+      <c r="F37" s="4" t="n">
+        <v>35536</v>
+      </c>
+      <c r="G37" s="4" t="inlineStr"/>
+      <c r="H37" s="4" t="n">
+        <v>605</v>
+      </c>
+      <c r="I37" s="4" t="n">
+        <v>658</v>
+      </c>
+      <c r="J37" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="K37" s="4" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B38" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="inlineStr">
+        <is>
+          <t>Saida: Back to School/ Promosi Ahli [10/02]</t>
+        </is>
+      </c>
+      <c r="E38" s="4" t="inlineStr"/>
+      <c r="F38" s="4" t="n">
+        <v>3253</v>
+      </c>
+      <c r="G38" s="4" t="inlineStr"/>
+      <c r="H38" s="4" t="n">
+        <v>326</v>
+      </c>
+      <c r="I38" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="K38" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>Wana: Grocery Shopping with 2 Kids [15/02]</t>
+        </is>
+      </c>
+      <c r="E39" s="4" t="inlineStr"/>
+      <c r="F39" s="4" t="n">
+        <v>2186</v>
+      </c>
+      <c r="G39" s="4" t="inlineStr"/>
+      <c r="H39" s="4" t="n">
+        <v>127</v>
+      </c>
+      <c r="I39" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="K39" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>Nina: Cucur Udang Rangup [24/02]</t>
+        </is>
+      </c>
+      <c r="E40" s="4" t="inlineStr"/>
+      <c r="F40" s="4" t="n">
+        <v>42767</v>
+      </c>
+      <c r="G40" s="4" t="inlineStr"/>
+      <c r="H40" s="4" t="n">
+        <v>694</v>
+      </c>
+      <c r="I40" s="4" t="n">
+        <v>299</v>
+      </c>
+      <c r="J40" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="K40" s="4" t="n">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="B27" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="inlineStr">
+      <c r="B41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="inlineStr">
         <is>
           <t>Post</t>
         </is>
       </c>
-      <c r="D27" s="3" t="inlineStr">
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>Selamat Hari Valentine
+[05/02]</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="n">
+        <v>93349</v>
+      </c>
+      <c r="F41" s="4" t="inlineStr"/>
+      <c r="G41" s="4" t="n">
+        <v>4147</v>
+      </c>
+      <c r="H41" s="4" t="n">
+        <v>538</v>
+      </c>
+      <c r="I41" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="J41" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K41" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="inlineStr">
         <is>
           <t>Cahaya Ramadan
 [24/02]</t>
         </is>
       </c>
-      <c r="E27" s="4" t="n">
-        <v>93349</v>
-      </c>
-      <c r="F27" s="4" t="inlineStr"/>
-      <c r="G27" s="4" t="n">
-        <v>4147</v>
-      </c>
-      <c r="H27" s="4" t="n">
-        <v>538</v>
-      </c>
-      <c r="I27" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="J27" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K27" s="4" t="n">
+      <c r="E42" s="4" t="n">
+        <v>151263</v>
+      </c>
+      <c r="F42" s="4" t="inlineStr"/>
+      <c r="G42" s="4" t="n">
+        <v>33779</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>965</v>
+      </c>
+      <c r="I42" s="4" t="n">
+        <v>232</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="K42" s="4" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="B43" s="2" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
-        <v>79</v>
-      </c>
-      <c r="B28" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C28" s="2" t="inlineStr">
+      <c r="C43" s="2" t="inlineStr">
         <is>
           <t>Post</t>
         </is>
       </c>
-      <c r="D28" s="3" t="inlineStr">
+      <c r="D43" s="3" t="inlineStr">
         <is>
           <t>Tawaran Istimewa 4 Hari [26/02]</t>
         </is>
       </c>
-      <c r="E28" s="4" t="n">
+      <c r="E43" s="4" t="n">
         <v>138367</v>
       </c>
-      <c r="F28" s="4" t="inlineStr"/>
-      <c r="G28" s="4" t="n">
+      <c r="F43" s="4" t="inlineStr"/>
+      <c r="G43" s="4" t="n">
         <v>10707</v>
       </c>
-      <c r="H28" s="4" t="n">
+      <c r="H43" s="4" t="n">
         <v>541</v>
       </c>
-      <c r="I28" s="4" t="n">
+      <c r="I43" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="J28" s="4" t="n">
+      <c r="J43" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="K28" s="4" t="n">
+      <c r="K43" s="4" t="n">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K28"/>
+  <autoFilter ref="A1:K43"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Processor logic working. Implementing UI UX design for app exporting
</commit_message>
<xml_diff>
--- a/output/marchmarketing_summary.xlsx
+++ b/output/marchmarketing_summary.xlsx
@@ -9,9 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Posts" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$K$43</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -19,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,6 +31,10 @@
     <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <color rgb="000563C1"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="3">
@@ -67,19 +69,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -458,7 +461,7 @@
     <col width="7" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
-    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="58" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
@@ -466,6 +469,7 @@
     <col width="8" customWidth="1" min="9" max="9"/>
     <col width="10" customWidth="1" min="10" max="10"/>
     <col width="7" customWidth="1" min="11" max="11"/>
+    <col width="44" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -524,6 +528,11 @@
           <t>Saved</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -561,6 +570,7 @@
       <c r="K2" s="4" t="n">
         <v>36</v>
       </c>
+      <c r="L2" s="3" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -596,6 +606,7 @@
       <c r="K3" s="4" t="n">
         <v>3</v>
       </c>
+      <c r="L3" s="3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -633,6 +644,7 @@
       <c r="K4" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="L4" s="3" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -671,6 +683,7 @@
       <c r="K5" s="4" t="n">
         <v>11</v>
       </c>
+      <c r="L5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -706,6 +719,7 @@
       <c r="K6" s="4" t="n">
         <v>16</v>
       </c>
+      <c r="L6" s="3" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -743,51 +757,50 @@
       <c r="K7" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="L7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>Weekend Shopping Spree 
-[03/02]</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>11692</v>
-      </c>
-      <c r="F8" s="4" t="inlineStr"/>
-      <c r="G8" s="4" t="n">
-        <v>1008</v>
-      </c>
+          <t>Promo Video: Cahaya Ramadan [26/02]</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr"/>
+      <c r="F8" s="4" t="n">
+        <v>51012</v>
+      </c>
+      <c r="G8" s="4" t="inlineStr"/>
       <c r="H8" s="4" t="n">
-        <v>1000</v>
+        <v>74</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="4" t="n">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L8" s="3" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
@@ -796,21 +809,22 @@
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>Loyalty Program (Gorme Omura Knife Series) [11/02]</t>
+          <t>Weekend Shopping Spree 
+[03/02]</t>
         </is>
       </c>
       <c r="E9" s="4" t="n">
-        <v>12157</v>
+        <v>11692</v>
       </c>
       <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" s="4" t="n">
-        <v>1002</v>
+        <v>1008</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>952</v>
+        <v>1000</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9" s="4" t="n">
         <v>0</v>
@@ -818,13 +832,14 @@
       <c r="K9" s="4" t="n">
         <v>5</v>
       </c>
+      <c r="L9" s="3" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
@@ -833,144 +848,150 @@
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>Daily Essential Grab 
-[17/02]</t>
+          <t>Loyalty Program (Gorme Omura Knife Series) [11/02]</t>
         </is>
       </c>
       <c r="E10" s="4" t="n">
-        <v>12450</v>
+        <v>12157</v>
       </c>
       <c r="F10" s="4" t="inlineStr"/>
       <c r="G10" s="4" t="n">
-        <v>1025</v>
+        <v>1002</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>1021</v>
+        <v>952</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="4" t="n">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="L10" s="3" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>Daily Essential Grab 
+[17/02]</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>12450</v>
+      </c>
+      <c r="F11" s="4" t="inlineStr"/>
+      <c r="G11" s="4" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>1021</v>
+      </c>
+      <c r="I11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="L11" s="3" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>Post</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>Loyalty Program (Gorme Omura Knife Series) [25/02]</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>12913</v>
+      </c>
+      <c r="F12" s="4" t="inlineStr"/>
+      <c r="G12" s="4" t="n">
+        <v>1023</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>1017</v>
+      </c>
+      <c r="I12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="L12" s="3" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
         <is>
           <t>Promo Cahaya Ramadan
 [26/02]</t>
         </is>
       </c>
-      <c r="E11" s="4" t="n">
-        <v>12913</v>
-      </c>
-      <c r="F11" s="4" t="inlineStr"/>
-      <c r="G11" s="4" t="n">
-        <v>1023</v>
-      </c>
-      <c r="H11" s="4" t="n">
-        <v>1017</v>
-      </c>
-      <c r="I11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Quesha Back To School Promo [03/02]</t>
-        </is>
-      </c>
-      <c r="E12" s="4" t="inlineStr"/>
-      <c r="F12" s="4" t="n">
-        <v>17343</v>
-      </c>
-      <c r="G12" s="4" t="inlineStr"/>
-      <c r="H12" s="4" t="n">
-        <v>180</v>
-      </c>
-      <c r="I12" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J12" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K12" s="4" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>Video</t>
-        </is>
-      </c>
-      <c r="D13" s="3" t="inlineStr">
-        <is>
-          <t>KOL TikTok – Nina Tomyam Seafood Recipe [07/02]</t>
-        </is>
-      </c>
       <c r="E13" s="4" t="inlineStr"/>
       <c r="F13" s="4" t="n">
-        <v>19125</v>
+        <v>35810</v>
       </c>
       <c r="G13" s="4" t="inlineStr"/>
       <c r="H13" s="4" t="n">
-        <v>461</v>
+        <v>18</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J13" s="4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K13" s="4" t="n">
-        <v>50</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
@@ -979,33 +1000,34 @@
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>KOL TikTok – Saida Back To School / Promosi Ahli [10/02]</t>
+          <t>KOL TikTok – Quesha Back To School Promo [03/02]</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr"/>
       <c r="F14" s="4" t="n">
-        <v>22053</v>
+        <v>17343</v>
       </c>
       <c r="G14" s="4" t="inlineStr"/>
       <c r="H14" s="4" t="n">
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J14" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="4" t="n">
-        <v>7</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="L14" s="3" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
@@ -1014,33 +1036,34 @@
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>KOL TikTok – Anne Weekend Groceries Shopping [10/02]</t>
+          <t>KOL TikTok – Nina Tomyam Seafood Recipe [07/02]</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr"/>
       <c r="F15" s="4" t="n">
-        <v>28764</v>
+        <v>19125</v>
       </c>
       <c r="G15" s="4" t="inlineStr"/>
       <c r="H15" s="4" t="n">
-        <v>115</v>
+        <v>461</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J15" s="4" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K15" s="4" t="n">
-        <v>12</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="L15" s="3" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
@@ -1049,33 +1072,34 @@
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>TikTok ASMR – Restock Pantry [14/02]</t>
+          <t>KOL TikTok – Saida Back To School / Promosi Ahli [10/02]</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr"/>
       <c r="F16" s="4" t="n">
-        <v>23571</v>
+        <v>22053</v>
       </c>
       <c r="G16" s="4" t="inlineStr"/>
       <c r="H16" s="4" t="n">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="I16" s="4" t="n">
         <v>1</v>
       </c>
       <c r="J16" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" s="4" t="n">
-        <v>9</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L16" s="3" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
@@ -1084,33 +1108,34 @@
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>KOL TikTok – Wana Grocery Shopping with 2 Kids [17/02]</t>
+          <t>KOL TikTok – Anne Weekend Groceries Shopping [10/02]</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr"/>
       <c r="F17" s="4" t="n">
-        <v>23214</v>
+        <v>28764</v>
       </c>
       <c r="G17" s="4" t="inlineStr"/>
       <c r="H17" s="4" t="n">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J17" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K17" s="4" t="n">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="L17" s="3" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
@@ -1119,33 +1144,34 @@
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>TikTok Video – Dua Lipa Trend [24/02]</t>
+          <t>TikTok ASMR – Restock Pantry [14/02]</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr"/>
       <c r="F18" s="4" t="n">
-        <v>45424</v>
+        <v>23571</v>
       </c>
       <c r="G18" s="4" t="inlineStr"/>
       <c r="H18" s="4" t="n">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="I18" s="4" t="n">
         <v>1</v>
       </c>
       <c r="J18" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18" s="4" t="n">
-        <v>15</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="L18" s="3" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
@@ -1154,33 +1180,34 @@
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>KOL TikTok – Nina Cucur Udang Rangup [24/02]</t>
+          <t>KOL TikTok – Wana Grocery Shopping with 2 Kids [17/02]</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr"/>
       <c r="F19" s="4" t="n">
-        <v>12631</v>
+        <v>23214</v>
       </c>
       <c r="G19" s="4" t="inlineStr"/>
       <c r="H19" s="4" t="n">
-        <v>382</v>
+        <v>69</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J19" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K19" s="4" t="n">
-        <v>50</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="L19" s="3" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
@@ -1189,142 +1216,144 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>TikTok Video – TFVM ada Produk Sendiri [26/02]</t>
+          <t>TikTok Video – Dua Lipa Trend [24/02]</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr"/>
       <c r="F20" s="4" t="n">
-        <v>22018</v>
+        <v>45424</v>
       </c>
       <c r="G20" s="4" t="inlineStr"/>
       <c r="H20" s="4" t="n">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J20" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K20" s="4" t="n">
-        <v>2</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="L20" s="3" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>Weekend Shopping Spree [03/02]</t>
-        </is>
-      </c>
-      <c r="E21" s="4" t="n">
-        <v>49275</v>
-      </c>
-      <c r="F21" s="4" t="inlineStr"/>
-      <c r="G21" s="4" t="n">
-        <v>4306</v>
-      </c>
+          <t>KOL TikTok – Nina Cucur Udang Rangup [24/02]</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr"/>
+      <c r="F21" s="4" t="n">
+        <v>12631</v>
+      </c>
+      <c r="G21" s="4" t="inlineStr"/>
       <c r="H21" s="4" t="n">
-        <v>237</v>
+        <v>382</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" s="4" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K21" s="4" t="n">
-        <v>21</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="L21" s="3" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>TikTok Video – TFVM ada Produk Sendiri [26/02]</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="inlineStr"/>
+      <c r="F22" s="4" t="n">
+        <v>22018</v>
+      </c>
+      <c r="G22" s="4" t="inlineStr"/>
+      <c r="H22" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="J22" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>Weekend Shopping Spree [03/02]</t>
-        </is>
-      </c>
-      <c r="E22" s="4" t="n">
-        <v>41113</v>
-      </c>
-      <c r="F22" s="4" t="inlineStr"/>
-      <c r="G22" s="4" t="n">
-        <v>3558</v>
-      </c>
-      <c r="H22" s="4" t="n">
-        <v>206</v>
-      </c>
-      <c r="I22" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="J22" s="4" t="n">
-        <v>1</v>
-      </c>
       <c r="K22" s="4" t="n">
-        <v>20</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L22" s="3" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
         <v>25</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>Nina Tomyam Seafood Recipe [07/02]</t>
-        </is>
-      </c>
-      <c r="E23" s="4" t="inlineStr"/>
-      <c r="F23" s="4" t="n">
-        <v>131496</v>
-      </c>
-      <c r="G23" s="4" t="inlineStr"/>
+          <t>Weekend Shopping Spree [03/02]</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="n">
+        <v>49275</v>
+      </c>
+      <c r="F23" s="4" t="inlineStr"/>
+      <c r="G23" s="4" t="n">
+        <v>4306</v>
+      </c>
       <c r="H23" s="4" t="n">
-        <v>481</v>
+        <v>237</v>
       </c>
       <c r="I23" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="J23" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="K23" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="L23" s="3" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
         <v>25</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
@@ -1333,35 +1362,36 @@
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>Loyalty Program – Gorme Omura Knife Series [11/02]</t>
+          <t>Weekend Shopping Spree [03/02]</t>
         </is>
       </c>
       <c r="E24" s="4" t="n">
-        <v>47133</v>
+        <v>41113</v>
       </c>
       <c r="F24" s="4" t="inlineStr"/>
       <c r="G24" s="4" t="n">
-        <v>4132</v>
+        <v>3558</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>496</v>
+        <v>206</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J24" s="4" t="n">
         <v>1</v>
       </c>
       <c r="K24" s="4" t="n">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="L24" s="3" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
         <v>25</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
@@ -1370,358 +1400,370 @@
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>Loyalty Program – Gorme Omura Knife Series [11/02]</t>
+          <t>Nina Tomyam Seafood Recipe [07/02]</t>
         </is>
       </c>
       <c r="E25" s="4" t="n">
-        <v>44547</v>
+        <v>47133</v>
       </c>
       <c r="F25" s="4" t="inlineStr"/>
       <c r="G25" s="4" t="n">
-        <v>3408</v>
+        <v>4132</v>
       </c>
       <c r="H25" s="4" t="n">
-        <v>470</v>
+        <v>496</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J25" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K25" s="4" t="n">
-        <v>4</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L25" s="3" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>TikTok ASMR – Restock Pantry [14/02]</t>
-        </is>
-      </c>
-      <c r="E26" s="4" t="inlineStr"/>
-      <c r="F26" s="4" t="n">
-        <v>51093</v>
-      </c>
-      <c r="G26" s="4" t="inlineStr"/>
+          <t>Loyalty Program – Gorme Omura Knife Series [11/02]</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>44547</v>
+      </c>
+      <c r="F26" s="4" t="inlineStr"/>
+      <c r="G26" s="4" t="n">
+        <v>3408</v>
+      </c>
       <c r="H26" s="4" t="n">
-        <v>81</v>
+        <v>470</v>
       </c>
       <c r="I26" s="4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J26" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K26" s="4" t="n">
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="L26" s="3" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>Daily Essential Grab [22/02]</t>
-        </is>
-      </c>
-      <c r="E27" s="4" t="n">
-        <v>40740</v>
-      </c>
-      <c r="F27" s="4" t="inlineStr"/>
-      <c r="G27" s="4" t="n">
-        <v>3350</v>
-      </c>
+          <t>Loyalty Program – Gorme Omura Knife Series [11/02]</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr"/>
+      <c r="F27" s="4" t="n">
+        <v>131496</v>
+      </c>
+      <c r="G27" s="4" t="inlineStr"/>
       <c r="H27" s="4" t="n">
-        <v>88</v>
+        <v>481</v>
       </c>
       <c r="I27" s="4" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J27" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K27" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="L27" s="3" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>Daily Essential Grab [22/02]</t>
-        </is>
-      </c>
-      <c r="E28" s="4" t="n">
-        <v>42339</v>
-      </c>
-      <c r="F28" s="4" t="inlineStr"/>
-      <c r="G28" s="4" t="n">
-        <v>3425</v>
-      </c>
+          <t>TikTok ASMR – Restock Pantry [14/02]</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="inlineStr"/>
+      <c r="F28" s="4" t="n">
+        <v>51093</v>
+      </c>
+      <c r="G28" s="4" t="inlineStr"/>
       <c r="H28" s="4" t="n">
-        <v>184</v>
+        <v>81</v>
       </c>
       <c r="I28" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J28" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="L28" s="3" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
         <v>26</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>Nina – Cucur Udang Rangup [24/02]</t>
-        </is>
-      </c>
-      <c r="E29" s="4" t="inlineStr"/>
-      <c r="F29" s="4" t="n">
-        <v>50440</v>
-      </c>
-      <c r="G29" s="4" t="inlineStr"/>
+          <t>Daily Essential Grab [22/02]</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="n">
+        <v>40740</v>
+      </c>
+      <c r="F29" s="4" t="inlineStr"/>
+      <c r="G29" s="4" t="n">
+        <v>3350</v>
+      </c>
       <c r="H29" s="4" t="n">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="I29" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29" s="4" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="4" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L29" s="3" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
         <v>26</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>TikTok Video – Dua Lipa Trend [24/02]</t>
-        </is>
-      </c>
-      <c r="E30" s="4" t="inlineStr"/>
-      <c r="F30" s="4" t="n">
-        <v>50719</v>
-      </c>
-      <c r="G30" s="4" t="inlineStr"/>
+          <t>Daily Essential Grab [22/02]</t>
+        </is>
+      </c>
+      <c r="E30" s="4" t="n">
+        <v>42339</v>
+      </c>
+      <c r="F30" s="4" t="inlineStr"/>
+      <c r="G30" s="4" t="n">
+        <v>3425</v>
+      </c>
       <c r="H30" s="4" t="n">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="I30" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J30" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="L30" s="3" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>Loyalty Program – Gorme Omura Knife Series [25/02]</t>
-        </is>
-      </c>
-      <c r="E31" s="4" t="n">
-        <v>41788</v>
-      </c>
-      <c r="F31" s="4" t="inlineStr"/>
-      <c r="G31" s="4" t="n">
-        <v>4215</v>
-      </c>
+          <t>Nina – Cucur Udang Rangup [24/02]</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="inlineStr"/>
+      <c r="F31" s="4" t="n">
+        <v>50440</v>
+      </c>
+      <c r="G31" s="4" t="inlineStr"/>
       <c r="H31" s="4" t="n">
-        <v>268</v>
+        <v>33</v>
       </c>
       <c r="I31" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K31" s="4" t="n">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L31" s="3" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>Loyalty Program – Gorme Omura Knife Series [25/02]</t>
-        </is>
-      </c>
-      <c r="E32" s="4" t="n">
-        <v>42824</v>
-      </c>
-      <c r="F32" s="4" t="inlineStr"/>
-      <c r="G32" s="4" t="n">
-        <v>3395</v>
-      </c>
+          <t>TikTok Video – Dua Lipa Trend [24/02]</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="inlineStr"/>
+      <c r="F32" s="4" t="n">
+        <v>50719</v>
+      </c>
+      <c r="G32" s="4" t="inlineStr"/>
       <c r="H32" s="4" t="n">
-        <v>353</v>
+        <v>8</v>
       </c>
       <c r="I32" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J32" s="4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K32" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="L32" s="3" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
         <v>27</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>TikTok Video – TFVM ada Produk Sendiri [26/02]</t>
-        </is>
-      </c>
-      <c r="E33" s="4" t="inlineStr"/>
-      <c r="F33" s="4" t="n">
-        <v>50582</v>
-      </c>
-      <c r="G33" s="4" t="inlineStr"/>
+          <t>Loyalty Program – Gorme Omura Knife Series [25/02]</t>
+        </is>
+      </c>
+      <c r="E33" s="4" t="n">
+        <v>41788</v>
+      </c>
+      <c r="F33" s="4" t="inlineStr"/>
+      <c r="G33" s="4" t="n">
+        <v>4215</v>
+      </c>
       <c r="H33" s="4" t="n">
-        <v>34</v>
+        <v>268</v>
       </c>
       <c r="I33" s="4" t="n">
         <v>1</v>
       </c>
       <c r="J33" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K33" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="L33" s="3" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
         <v>27</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>Promo Video: Cahaya Ramadan [26/02]</t>
-        </is>
-      </c>
-      <c r="E34" s="4" t="inlineStr"/>
-      <c r="F34" s="4" t="n">
-        <v>51285</v>
-      </c>
-      <c r="G34" s="4" t="inlineStr"/>
+          <t>Loyalty Program – Gorme Omura Knife Series [25/02]</t>
+        </is>
+      </c>
+      <c r="E34" s="4" t="n">
+        <v>42824</v>
+      </c>
+      <c r="F34" s="4" t="inlineStr"/>
+      <c r="G34" s="4" t="n">
+        <v>3395</v>
+      </c>
       <c r="H34" s="4" t="n">
-        <v>23</v>
+        <v>353</v>
       </c>
       <c r="I34" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J34" s="4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K34" s="4" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L34" s="3" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
         <v>27</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
@@ -1730,19 +1772,19 @@
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>Promo Video: Cahaya Ramadan [26/02]</t>
+          <t>TikTok Video – TFVM ada Produk Sendiri [26/02]</t>
         </is>
       </c>
       <c r="E35" s="4" t="inlineStr"/>
       <c r="F35" s="4" t="n">
-        <v>50209</v>
+        <v>50582</v>
       </c>
       <c r="G35" s="4" t="inlineStr"/>
       <c r="H35" s="4" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I35" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="4" t="n">
         <v>0</v>
@@ -1750,13 +1792,14 @@
       <c r="K35" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="L35" s="3" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
@@ -1765,33 +1808,34 @@
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>Quesha: Back to School [03/02]</t>
+          <t>Promo Video: Cahaya Ramadan [26/02]</t>
         </is>
       </c>
       <c r="E36" s="4" t="inlineStr"/>
       <c r="F36" s="4" t="n">
-        <v>10307</v>
+        <v>51285</v>
       </c>
       <c r="G36" s="4" t="inlineStr"/>
       <c r="H36" s="4" t="n">
-        <v>225</v>
+        <v>23</v>
       </c>
       <c r="I36" s="4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J36" s="4" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="K36" s="4" t="n">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L36" s="3" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
@@ -1800,30 +1844,31 @@
       </c>
       <c r="D37" s="3" t="inlineStr">
         <is>
-          <t>Nina: Tomyam Seafood Recipe [07/02]</t>
+          <t>Promo Video: Cahaya Ramadan [26/02]</t>
         </is>
       </c>
       <c r="E37" s="4" t="inlineStr"/>
       <c r="F37" s="4" t="n">
-        <v>35536</v>
+        <v>50209</v>
       </c>
       <c r="G37" s="4" t="inlineStr"/>
       <c r="H37" s="4" t="n">
-        <v>605</v>
+        <v>30</v>
       </c>
       <c r="I37" s="4" t="n">
-        <v>658</v>
+        <v>0</v>
       </c>
       <c r="J37" s="4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K37" s="4" t="n">
-        <v>252</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L37" s="3" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>1</v>
@@ -1835,30 +1880,35 @@
       </c>
       <c r="D38" s="3" t="inlineStr">
         <is>
-          <t>Saida: Back to School/ Promosi Ahli [10/02]</t>
+          <t>Quesha: Back to School [03/02]</t>
         </is>
       </c>
       <c r="E38" s="4" t="inlineStr"/>
       <c r="F38" s="4" t="n">
-        <v>3253</v>
+        <v>10307</v>
       </c>
       <c r="G38" s="4" t="inlineStr"/>
       <c r="H38" s="4" t="n">
-        <v>326</v>
+        <v>225</v>
       </c>
       <c r="I38" s="4" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="J38" s="4" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="K38" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="L38" s="5" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DFmlwmaTHdI</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>2</v>
@@ -1870,25 +1920,30 @@
       </c>
       <c r="D39" s="3" t="inlineStr">
         <is>
-          <t>Wana: Grocery Shopping with 2 Kids [15/02]</t>
+          <t>Nina: Tomyam Seafood Recipe [07/02]</t>
         </is>
       </c>
       <c r="E39" s="4" t="inlineStr"/>
       <c r="F39" s="4" t="n">
-        <v>2186</v>
+        <v>35536</v>
       </c>
       <c r="G39" s="4" t="inlineStr"/>
       <c r="H39" s="4" t="n">
-        <v>127</v>
+        <v>605</v>
       </c>
       <c r="I39" s="4" t="n">
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="J39" s="4" t="n">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="K39" s="4" t="n">
-        <v>1</v>
+        <v>252</v>
+      </c>
+      <c r="L39" s="5" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DFws0PizSyc</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1896,7 +1951,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
@@ -1905,101 +1960,110 @@
       </c>
       <c r="D40" s="3" t="inlineStr">
         <is>
-          <t>Nina: Cucur Udang Rangup [24/02]</t>
+          <t>Saida: Back to School/ Promosi Ahli [10/02]</t>
         </is>
       </c>
       <c r="E40" s="4" t="inlineStr"/>
       <c r="F40" s="4" t="n">
-        <v>42767</v>
+        <v>3253</v>
       </c>
       <c r="G40" s="4" t="inlineStr"/>
       <c r="H40" s="4" t="n">
-        <v>694</v>
+        <v>326</v>
       </c>
       <c r="I40" s="4" t="n">
-        <v>299</v>
+        <v>22</v>
       </c>
       <c r="J40" s="4" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="K40" s="4" t="n">
-        <v>791</v>
+        <v>4</v>
+      </c>
+      <c r="L40" s="5" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DF4rOJ5pd-b</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
         <is>
-          <t>Selamat Hari Valentine
-[05/02]</t>
-        </is>
-      </c>
-      <c r="E41" s="4" t="n">
-        <v>93349</v>
-      </c>
-      <c r="F41" s="4" t="inlineStr"/>
-      <c r="G41" s="4" t="n">
-        <v>4147</v>
-      </c>
+          <t>Wana: Grocery Shopping with 2 Kids [15/02]</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="inlineStr"/>
+      <c r="F41" s="4" t="n">
+        <v>2186</v>
+      </c>
+      <c r="G41" s="4" t="inlineStr"/>
       <c r="H41" s="4" t="n">
-        <v>538</v>
+        <v>127</v>
       </c>
       <c r="I41" s="4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J41" s="4" t="n">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="K41" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="L41" s="5" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DGFt7mBy5Rf</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
         <is>
-          <t>Cahaya Ramadan
-[24/02]</t>
-        </is>
-      </c>
-      <c r="E42" s="4" t="n">
-        <v>151263</v>
-      </c>
-      <c r="F42" s="4" t="inlineStr"/>
-      <c r="G42" s="4" t="n">
-        <v>33779</v>
-      </c>
+          <t>Nina: Cucur Udang Rangup [24/02]</t>
+        </is>
+      </c>
+      <c r="E42" s="4" t="inlineStr"/>
+      <c r="F42" s="4" t="n">
+        <v>42767</v>
+      </c>
+      <c r="G42" s="4" t="inlineStr"/>
       <c r="H42" s="4" t="n">
-        <v>965</v>
+        <v>694</v>
       </c>
       <c r="I42" s="4" t="n">
-        <v>232</v>
+        <v>299</v>
       </c>
       <c r="J42" s="4" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="K42" s="4" t="n">
-        <v>29</v>
+        <v>791</v>
+      </c>
+      <c r="L42" s="5" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DGdSCbmTSKZ</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -2007,7 +2071,7 @@
         <v>79</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
@@ -2016,31 +2080,116 @@
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>Tawaran Istimewa 4 Hari [26/02]</t>
+          <t>Selamat Hari Valentine
+[05/02]</t>
         </is>
       </c>
       <c r="E43" s="4" t="n">
-        <v>138367</v>
+        <v>93349</v>
       </c>
       <c r="F43" s="4" t="inlineStr"/>
       <c r="G43" s="4" t="n">
+        <v>4147</v>
+      </c>
+      <c r="H43" s="4" t="n">
+        <v>538</v>
+      </c>
+      <c r="I43" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="J43" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K43" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="L43" s="3" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>Cahaya Ramadan
+[24/02]</t>
+        </is>
+      </c>
+      <c r="E44" s="4" t="n">
+        <v>151263</v>
+      </c>
+      <c r="F44" s="4" t="inlineStr"/>
+      <c r="G44" s="4" t="n">
+        <v>33779</v>
+      </c>
+      <c r="H44" s="4" t="n">
+        <v>965</v>
+      </c>
+      <c r="I44" s="4" t="n">
+        <v>232</v>
+      </c>
+      <c r="J44" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="K44" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="L44" s="3" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="D45" s="3" t="inlineStr">
+        <is>
+          <t>Tawaran Istimewa 4 Hari [26/02]</t>
+        </is>
+      </c>
+      <c r="E45" s="4" t="n">
+        <v>138367</v>
+      </c>
+      <c r="F45" s="4" t="inlineStr"/>
+      <c r="G45" s="4" t="n">
         <v>10707</v>
       </c>
-      <c r="H43" s="4" t="n">
+      <c r="H45" s="4" t="n">
         <v>541</v>
       </c>
-      <c r="I43" s="4" t="n">
+      <c r="I45" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="J43" s="4" t="n">
+      <c r="J45" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="K43" s="4" t="n">
+      <c r="K45" s="4" t="n">
         <v>4</v>
       </c>
+      <c r="L45" s="3" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K43"/>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L38" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L39" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L40" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L41" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L42" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>